<commit_message>
Added sample data for MAS consolidated
</commit_message>
<xml_diff>
--- a/data_capture/static/data_capture/Price_Proposal_Template_SERVICES_AND_TRAINING_FINAL.xlsx
+++ b/data_capture/static/data_capture/Price_Proposal_Template_SERVICES_AND_TRAINING_FINAL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t xml:space="preserve">Vendor Name*</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">SIN/SIN Proposed*</t>
   </si>
   <si>
-    <t xml:space="preserve">Service Proposed  (eg Job Title/Task)*</t>
+    <t xml:space="preserve">Service Proposed (eg Job Title/Task)*</t>
   </si>
   <si>
     <t xml:space="preserve">Description*
@@ -87,16 +87,55 @@
     <t xml:space="preserve">Supporting Invoice or Document Number(Initial submittal)*</t>
   </si>
   <si>
-    <t xml:space="preserve">712-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High School</t>
+    <t xml:space="preserve">XYZ, INC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">874-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recognized as a subject matter expert with relevant experience which includes, but is not limited to, supporting large business process improvement and management consulting projects related to the individual’s subject matter expertise. These senior personnel are recognized experts in functional domains (e.g., finance, business administration, etc.) with years of direct experience. They have extensive experience as organizational leaders and senior Project Managers and can manage multiple programs and projects. They are familiar with state-of-the art advances in their subject area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process improvement, finance, senior project manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market</t>
   </si>
   <si>
     <t xml:space="preserve">Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applies specific knowledge to the identification of business problems and contributes to the recommendation of solutions; can lead small task teams in project sub-components. Collects and analyzes data to provide support to all business functions. Uses structured analysis techniques to define business process support requirements. Analyzes and documents support requirements and develops appropriate support data. Assists in the development and/or production of supporting documentation. Develops procedures to record and track data to facilitate internal management reviews and project activities. Ensures effective data flow on projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data management, small teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market </t>
   </si>
 </sst>
 </file>
@@ -110,7 +149,7 @@
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -151,6 +190,13 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -216,11 +262,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +316,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,22 +408,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="71.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="46.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.71"/>
@@ -379,96 +441,168 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+    <row r="2" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="D2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="G2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="0" t="n">
-        <v>10.2</v>
+        <v>10</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="16" t="n">
+        <v>200</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="16" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>